<commit_message>
excluindo calc errada do felipe
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicho\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/831f5f1da6d5c7f7/Área de Trabalho/Luminous BD/Projeto-Luminous-BD/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{B0A05620-D061-42A5-BFDA-06A2800CCCB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
@@ -935,8 +935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34115E4B-87B5-4FBF-AA14-8031D9C8B86B}">
   <dimension ref="E1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>